<commit_message>
rerun scraper, new data
</commit_message>
<xml_diff>
--- a/week-5/Regular Expression and Text Proccessing/plantbook.xlsx
+++ b/week-5/Regular Expression and Text Proccessing/plantbook.xlsx
@@ -1887,7 +1887,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3691,7 +3691,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -3911,7 +3911,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>plant, combo</t>
+          <t>combo, plant</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">

</xml_diff>